<commit_message>
Adicionado todos os cenarios de testes, junto com os reportes e hooks.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Documents\Projetos\Mobile\target\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Documents\projetoguardado\Mobile\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A93F43-E324-442D-9730-373DA2F58E67}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D07297-E9C2-4406-B4B3-15E5BB2AF883}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="16665" windowHeight="7065" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="5475" yWindow="2190" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Matheus</t>
   </si>
@@ -125,21 +125,12 @@
     <t>Spdasdasds</t>
   </si>
   <si>
-    <t>Headset</t>
-  </si>
-  <si>
-    <t>Tenis</t>
-  </si>
-  <si>
     <t>Headset H390</t>
   </si>
   <si>
     <t>Confirmar Senha</t>
   </si>
   <si>
-    <t>HP Pro</t>
-  </si>
-  <si>
     <t>laptop</t>
   </si>
   <si>
@@ -170,14 +161,29 @@
     <t>Maatthe0109</t>
   </si>
   <si>
-    <t>AmimT199</t>
+    <t>LOGITECH</t>
+  </si>
+  <si>
+    <t>HEADPHONES</t>
+  </si>
+  <si>
+    <t>HP ZBOOK</t>
+  </si>
+  <si>
+    <t>Laptops</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>LegoHeal4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +203,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -223,11 +236,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,7 +594,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -609,7 +623,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -649,7 +663,7 @@
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f ca="1">VLOOKUP(RANDBETWEEN(1,7),A8:B14,2,FALSE)</f>
-        <v>Arvore321</v>
+        <v>Futebol234</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -696,14 +710,14 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+        <v>34</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -711,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -719,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -727,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -735,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -743,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -751,7 +765,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +786,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,21 +797,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -814,9 +828,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91637A43-323E-4909-B4CF-65559BD2B712}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -826,15 +842,20 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="B2" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Alterado o metodo de falha do cenairo de criar conta, adicionado metodo para gerar um user name aleatorio automatico.
</commit_message>
<xml_diff>
--- a/target/Excel/Dados.xlsx
+++ b/target/Excel/Dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matheus.vieira\Documents\projetoguardado\Mobile\target\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D07297-E9C2-4406-B4B3-15E5BB2AF883}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE7DC14-FAD5-4A0E-9AD6-6B629E61C9EE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="2190" windowWidth="15375" windowHeight="7875" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{E0E69BFF-8C0C-4BBC-880E-E66347D52EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Contas" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Matheus</t>
   </si>
   <si>
-    <t>Vieira</t>
-  </si>
-  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -89,42 +86,12 @@
     <t>06695-480</t>
   </si>
   <si>
-    <t>Felipe</t>
-  </si>
-  <si>
-    <t>felipe.almeida@hotmail.com</t>
-  </si>
-  <si>
-    <t>Senha321</t>
-  </si>
-  <si>
-    <t>Almeida</t>
-  </si>
-  <si>
-    <t>(11)972450987</t>
-  </si>
-  <si>
-    <t>Taboão</t>
-  </si>
-  <si>
-    <t>Cesário Dau</t>
-  </si>
-  <si>
-    <t>Sp</t>
-  </si>
-  <si>
-    <t>04487-920</t>
-  </si>
-  <si>
     <t>Pais</t>
   </si>
   <si>
     <t>Brazil</t>
   </si>
   <si>
-    <t>Spdasdasds</t>
-  </si>
-  <si>
     <t>Headset H390</t>
   </si>
   <si>
@@ -137,30 +104,6 @@
     <t>HP Stream</t>
   </si>
   <si>
-    <t>Random</t>
-  </si>
-  <si>
-    <t>Fire12</t>
-  </si>
-  <si>
-    <t>Selu981</t>
-  </si>
-  <si>
-    <t>Barca132</t>
-  </si>
-  <si>
-    <t>Arvore321</t>
-  </si>
-  <si>
-    <t>Futebol234</t>
-  </si>
-  <si>
-    <t>Uirs</t>
-  </si>
-  <si>
-    <t>Maatthe0109</t>
-  </si>
-  <si>
     <t>LOGITECH</t>
   </si>
   <si>
@@ -176,7 +119,13 @@
     <t>Celular</t>
   </si>
   <si>
-    <t>LegoHeal4</t>
+    <t>Aleatorio</t>
+  </si>
+  <si>
+    <t>SaoPaulo</t>
+  </si>
+  <si>
+    <t>Amim</t>
   </si>
 </sst>
 </file>
@@ -560,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93621F3-1ABA-4547-8339-842847F49F65}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,126 +527,91 @@
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.7109375" customWidth="1"/>
     <col min="13" max="13" width="44.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
       </c>
       <c r="K2" t="s">
         <v>29</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f ca="1">VLOOKUP(RANDBETWEEN(1,7),A8:B14,2,FALSE)</f>
-        <v>Futebol234</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M4" s="2"/>
@@ -706,67 +620,10 @@
       <c r="J5" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -774,10 +631,9 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{D868038A-3265-4776-B616-35A1FE857EEF}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{348E6C8F-65C8-4DD2-BED7-A02BB8BDB3DD}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -785,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A469EE5-3D0C-467A-8AB5-81E170E63C51}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,21 +653,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -831,7 +687,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,15 +698,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1"/>
     </row>

</xml_diff>